<commit_message>
Adding Gitignore. Adding Story Points to stories assigned to me in Sprint 1
</commit_message>
<xml_diff>
--- a/TeamSSW55AgileMethodsCJBS_Report.xlsx
+++ b/TeamSSW55AgileMethodsCJBS_Report.xlsx
@@ -5,7 +5,7 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CCorr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CCorr\OneDrive\Documents\SSW555AgileMethodsCJBS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="218">
   <si>
     <t>Find marriage date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -726,6 +726,9 @@
   </si>
   <si>
     <t>https://github.com/jj1976/SSW555AgileMethodsCJBS</t>
+  </si>
+  <si>
+    <t>Story Points</t>
   </si>
 </sst>
 </file>
@@ -2152,10 +2155,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2165,9 +2168,10 @@
     <col min="3" max="3" width="28.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.625" customWidth="1"/>
     <col min="5" max="5" width="7.625" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
@@ -2183,8 +2187,11 @@
       <c r="E1" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2201,7 +2208,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2218,7 +2225,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>132</v>
       </c>
@@ -2226,7 +2233,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>133</v>
       </c>
@@ -2234,7 +2241,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>134</v>
       </c>
@@ -2242,7 +2249,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>135</v>
       </c>
@@ -2250,7 +2257,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>136</v>
       </c>
@@ -2258,7 +2265,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>137</v>
       </c>
@@ -2266,7 +2273,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>138</v>
       </c>
@@ -2274,7 +2281,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>139</v>
       </c>
@@ -2282,7 +2289,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>140</v>
       </c>
@@ -2290,7 +2297,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>141</v>
       </c>
@@ -2298,7 +2305,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>142</v>
       </c>
@@ -2306,7 +2313,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>143</v>
       </c>
@@ -2314,7 +2321,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>144</v>
       </c>
@@ -2322,7 +2329,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>145</v>
       </c>
@@ -2330,7 +2337,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>146</v>
       </c>
@@ -2338,7 +2345,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>147</v>
       </c>
@@ -2346,7 +2353,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>148</v>
       </c>
@@ -2354,7 +2361,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>149</v>
       </c>
@@ -2362,7 +2369,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2378,8 +2385,11 @@
       <c r="E22" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2396,7 +2406,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2413,7 +2423,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>153</v>
       </c>
@@ -2421,7 +2431,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -2437,8 +2447,11 @@
       <c r="E26" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>155</v>
       </c>
@@ -2446,7 +2459,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>156</v>
       </c>
@@ -2454,7 +2467,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>157</v>
       </c>
@@ -2462,7 +2475,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>158</v>
       </c>
@@ -2470,7 +2483,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>159</v>
       </c>
@@ -2478,7 +2491,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>160</v>
       </c>
@@ -3291,7 +3304,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>134</v>
       </c>
@@ -3302,7 +3315,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>135</v>
       </c>
@@ -3533,7 +3546,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>156</v>
       </c>

</xml_diff>

<commit_message>
latest code from master
</commit_message>
<xml_diff>
--- a/TeamSSW55AgileMethodsCJBS_Report.xlsx
+++ b/TeamSSW55AgileMethodsCJBS_Report.xlsx
@@ -5,11 +5,11 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacje17\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bvijayakumar\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="199">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1022,11 +1022,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="175679440"/>
-        <c:axId val="175683920"/>
+        <c:axId val="438822520"/>
+        <c:axId val="438823304"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="175679440"/>
+        <c:axId val="438822520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1036,14 +1036,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175683920"/>
+        <c:crossAx val="438823304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="175683920"/>
+        <c:axId val="438823304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1054,7 +1054,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175679440"/>
+        <c:crossAx val="438822520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1147,11 +1147,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="175686160"/>
-        <c:axId val="175686720"/>
+        <c:axId val="438821344"/>
+        <c:axId val="438823696"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="175686160"/>
+        <c:axId val="438821344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1161,14 +1161,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175686720"/>
+        <c:crossAx val="438823696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="175686720"/>
+        <c:axId val="438823696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1179,7 +1179,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175686160"/>
+        <c:crossAx val="438821344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1216,7 +1216,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1254,7 +1254,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1329,7 +1329,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1394,7 +1394,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1463,7 +1463,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1533,7 +1533,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1602,7 +1602,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1672,7 +1672,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2015,7 +2015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2132,8 +2132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2252,7 +2252,7 @@
         <v>183</v>
       </c>
       <c r="E8" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="F8">
         <v>3</v>
@@ -2288,7 +2288,7 @@
         <v>183</v>
       </c>
       <c r="E11" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="F11">
         <v>3</v>
@@ -2495,43 +2495,19 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>2</v>
-      </c>
       <c r="B31" t="s">
         <v>140</v>
       </c>
       <c r="C31" t="s">
         <v>96</v>
       </c>
-      <c r="D31" t="s">
-        <v>183</v>
-      </c>
-      <c r="E31" t="s">
-        <v>186</v>
-      </c>
-      <c r="F31">
-        <v>3</v>
-      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>2</v>
-      </c>
       <c r="B32" t="s">
         <v>141</v>
       </c>
       <c r="C32" t="s">
         <v>97</v>
-      </c>
-      <c r="D32" t="s">
-        <v>183</v>
-      </c>
-      <c r="E32" t="s">
-        <v>186</v>
-      </c>
-      <c r="F32">
-        <v>3</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.2">
@@ -2932,8 +2908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2942,9 +2918,9 @@
     <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="6.625" customWidth="1"/>
     <col min="5" max="5" width="9.875" customWidth="1"/>
-    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" customWidth="1"/>
+    <col min="7" max="7" width="6.625" customWidth="1"/>
+    <col min="8" max="8" width="7.625" customWidth="1"/>
     <col min="9" max="9" width="10.875" style="6"/>
   </cols>
   <sheetData>
@@ -3054,15 +3030,7 @@
       <c r="F4">
         <v>3</v>
       </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>197</v>
-      </c>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -3083,15 +3051,7 @@
       <c r="F5">
         <v>3</v>
       </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>197</v>
-      </c>
+      <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">

</xml_diff>

<commit_message>
Updating the report to the latest
</commit_message>
<xml_diff>
--- a/TeamSSW55AgileMethodsCJBS_Report.xlsx
+++ b/TeamSSW55AgileMethodsCJBS_Report.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10210"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bvijayakumar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ccorrado/PycharmProjects/SSW555AgileMethodsCJBS/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25700" windowHeight="14560" tabRatio="500" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -22,10 +22,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <definedNames>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-  </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -35,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="198">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -655,19 +652,16 @@
     <t>rsukitha</t>
   </si>
   <si>
-    <t>Est Time (hrs)</t>
-  </si>
-  <si>
-    <t>done</t>
-  </si>
-  <si>
-    <t>Done</t>
+    <t>Est Time</t>
+  </si>
+  <si>
+    <t>Code Velocity ( Loc/hr)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -681,31 +675,26 @@
       <b/>
       <sz val="10"/>
       <name val="Verdana"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Verdana"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="11"/>
       <name val="Verdana"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Cambria"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -902,36 +891,8 @@
     <cellStyle name="Hyperlink" xfId="65" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD7D7D7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="1"/>
-      <tableStyleElement type="headerRow" dxfId="0"/>
-    </tableStyle>
-  </tableStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -944,7 +905,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -970,22 +931,22 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>41675</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41682</c:v>
+                  <c:v>41689</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41689</c:v>
+                  <c:v>41703</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41696</c:v>
+                  <c:v>41717</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41703</c:v>
+                  <c:v>41731</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1006,7 +967,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F4F8-45B3-8E48-DE1D90C4942A}"/>
             </c:ext>
@@ -1022,28 +983,28 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="438822520"/>
-        <c:axId val="438823304"/>
+        <c:axId val="78186752"/>
+        <c:axId val="78188544"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="438822520"/>
+        <c:axId val="78186752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="438823304"/>
+        <c:crossAx val="78188544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="438823304"/>
+        <c:axId val="78188544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1054,7 +1015,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="438822520"/>
+        <c:crossAx val="78186752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1072,7 +1033,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1104,16 +1065,16 @@
                   <c:v>41675</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41682</c:v>
+                  <c:v>41689</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41689</c:v>
+                  <c:v>41703</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41696</c:v>
+                  <c:v>41717</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41703</c:v>
+                  <c:v>41731</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1127,11 +1088,14 @@
                 <c:pt idx="0">
                   <c:v>32</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6D39-4E3C-9231-02575099E635}"/>
             </c:ext>
@@ -1147,11 +1111,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="438821344"/>
-        <c:axId val="438823696"/>
+        <c:axId val="83934592"/>
+        <c:axId val="83960960"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="438821344"/>
+        <c:axId val="83934592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1161,14 +1125,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="438823696"/>
+        <c:crossAx val="83960960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="438823696"/>
+        <c:axId val="83960960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1179,7 +1143,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="438821344"/>
+        <c:crossAx val="83934592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1216,7 +1180,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1254,7 +1218,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1329,7 +1293,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1394,7 +1358,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1463,7 +1427,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1533,7 +1497,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1602,7 +1566,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1672,7 +1636,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2012,23 +1976,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="B1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2045,7 +2009,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>181</v>
       </c>
@@ -2059,7 +2023,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>177</v>
       </c>
@@ -2073,7 +2037,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>176</v>
       </c>
@@ -2087,7 +2051,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>173</v>
       </c>
@@ -2104,7 +2068,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="D8" s="4" t="s">
         <v>31</v>
       </c>
@@ -2118,10 +2082,10 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="D3" r:id="rId3"/>
-    <hyperlink ref="D4" r:id="rId4"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2129,24 +2093,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView topLeftCell="A19" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.625" customWidth="1"/>
-    <col min="5" max="5" width="7.625" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
     <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2166,7 +2130,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2179,14 +2143,14 @@
       <c r="D2" t="s">
         <v>173</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>198</v>
+      <c r="E2" t="s">
+        <v>186</v>
       </c>
       <c r="F2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2199,22 +2163,31 @@
       <c r="D3" t="s">
         <v>173</v>
       </c>
-      <c r="E3" s="17" t="s">
-        <v>198</v>
+      <c r="E3" t="s">
+        <v>186</v>
       </c>
       <c r="F3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>113</v>
       </c>
       <c r="C4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>174</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>114</v>
       </c>
@@ -2222,7 +2195,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>115</v>
       </c>
@@ -2230,7 +2203,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>116</v>
       </c>
@@ -2238,7 +2211,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2258,7 +2231,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
         <v>118</v>
       </c>
@@ -2266,7 +2239,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
         <v>119</v>
       </c>
@@ -2274,7 +2247,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2294,7 +2267,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
         <v>121</v>
       </c>
@@ -2302,7 +2275,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
         <v>122</v>
       </c>
@@ -2310,7 +2283,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>123</v>
       </c>
@@ -2318,7 +2291,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>124</v>
       </c>
@@ -2326,7 +2299,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
         <v>125</v>
       </c>
@@ -2334,7 +2307,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B17" t="s">
         <v>126</v>
       </c>
@@ -2342,7 +2315,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B18" t="s">
         <v>127</v>
       </c>
@@ -2350,7 +2323,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
         <v>128</v>
       </c>
@@ -2358,7 +2331,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
         <v>129</v>
       </c>
@@ -2366,7 +2339,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
         <v>130</v>
       </c>
@@ -2374,7 +2347,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2394,7 +2367,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2414,7 +2387,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2434,7 +2407,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B25" t="s">
         <v>134</v>
       </c>
@@ -2442,7 +2415,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>1</v>
       </c>
@@ -2462,7 +2435,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B27" t="s">
         <v>136</v>
       </c>
@@ -2470,7 +2443,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
         <v>137</v>
       </c>
@@ -2478,7 +2451,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B29" t="s">
         <v>138</v>
       </c>
@@ -2486,31 +2459,52 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30">
+        <v>2</v>
+      </c>
       <c r="B30" t="s">
         <v>139</v>
       </c>
       <c r="C30" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>174</v>
+      </c>
+      <c r="F30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31">
+        <v>2</v>
+      </c>
       <c r="B31" t="s">
         <v>140</v>
       </c>
       <c r="C31" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D31" s="17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32">
+        <v>2</v>
+      </c>
       <c r="B32" t="s">
         <v>141</v>
       </c>
       <c r="C32" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D32" s="17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B33" t="s">
         <v>142</v>
       </c>
@@ -2518,7 +2512,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B34" t="s">
         <v>143</v>
       </c>
@@ -2526,7 +2520,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B35" t="s">
         <v>144</v>
       </c>
@@ -2534,7 +2528,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B36" t="s">
         <v>145</v>
       </c>
@@ -2542,7 +2536,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B37" t="s">
         <v>146</v>
       </c>
@@ -2550,7 +2544,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B38" t="s">
         <v>147</v>
       </c>
@@ -2558,23 +2552,47 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A39">
+        <v>2</v>
+      </c>
       <c r="B39" t="s">
         <v>148</v>
       </c>
       <c r="C39" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D39" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A40">
+        <v>2</v>
+      </c>
       <c r="B40" t="s">
         <v>149</v>
       </c>
       <c r="C40" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D40" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B41" t="s">
         <v>150</v>
       </c>
@@ -2582,7 +2600,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B42" t="s">
         <v>151</v>
       </c>
@@ -2590,7 +2608,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B43" t="s">
         <v>152</v>
       </c>
@@ -2606,54 +2624,54 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A4" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="7"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>158</v>
       </c>
@@ -2676,7 +2694,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>159</v>
       </c>
@@ -2692,12 +2710,12 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>160</v>
       </c>
       <c r="B16" s="13">
-        <v>41682</v>
+        <v>41689</v>
       </c>
       <c r="C16" s="14">
         <v>24</v>
@@ -2717,12 +2735,12 @@
         <v>125.00000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
         <v>161</v>
       </c>
       <c r="B17" s="13">
-        <v>41689</v>
+        <v>41703</v>
       </c>
       <c r="C17" s="14"/>
       <c r="D17">
@@ -2740,12 +2758,12 @@
         <v>102.22222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
         <v>162</v>
       </c>
       <c r="B18" s="13">
-        <v>41696</v>
+        <v>41717</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18">
@@ -2763,12 +2781,12 @@
         <v>97.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
         <v>163</v>
       </c>
       <c r="B19" s="13">
-        <v>41703</v>
+        <v>41731</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19">
@@ -2794,24 +2812,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A4" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2828,10 +2846,10 @@
         <v>25</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>41675</v>
       </c>
@@ -2842,58 +2860,86 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
-        <v>41682</v>
+        <v>41689</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
       </c>
       <c r="C3">
         <f>B2-B3</f>
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="D3">
-        <v>250</v>
+        <f>Sprint1!G10</f>
+        <v>68</v>
       </c>
       <c r="E3">
-        <v>120</v>
+        <f>Sprint1!H10</f>
+        <v>535</v>
       </c>
       <c r="F3" s="9">
         <f>(D3-D2)/E3*60</f>
-        <v>125.00000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>7.6261682242990654</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="7">
-        <v>41689</v>
+        <v>41703</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>Sprint2!H10</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="9" t="e">
+        <f t="shared" ref="F4:F6" si="0">(D4-D3)/E4*60</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
-        <v>41696</v>
+        <v>41717</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5" si="0">B4-B5</f>
+        <f t="shared" ref="C5" si="1">B4-B5</f>
         <v>0</v>
       </c>
       <c r="D5">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>121</v>
-      </c>
-      <c r="F5" s="9">
-        <f t="shared" ref="F5" si="1">(D5-D4)/E5*60</f>
-        <v>123.96694214876032</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <f>Sprint3!H10</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="7">
-        <v>41703</v>
+        <v>41731</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>1000</v>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f>Sprint4!H10</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="9" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
@@ -2905,26 +2951,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.625" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.625" customWidth="1"/>
-    <col min="5" max="5" width="9.875" customWidth="1"/>
-    <col min="6" max="6" width="7.5" customWidth="1"/>
-    <col min="7" max="7" width="6.625" customWidth="1"/>
-    <col min="8" max="8" width="7.625" customWidth="1"/>
-    <col min="9" max="9" width="10.875" style="6"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2953,7 +2999,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>111</v>
       </c>
@@ -2967,22 +3013,13 @@
         <v>186</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -2996,22 +3033,13 @@
         <v>186</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>117</v>
       </c>
@@ -3025,14 +3053,20 @@
         <v>186</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>180</v>
+      </c>
+      <c r="G4">
+        <v>20</v>
+      </c>
+      <c r="H4">
+        <v>15</v>
       </c>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>120</v>
       </c>
@@ -3046,14 +3080,20 @@
         <v>186</v>
       </c>
       <c r="E5">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>120</v>
+      </c>
+      <c r="G5">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
       </c>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>131</v>
       </c>
@@ -3067,13 +3107,22 @@
         <v>186</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="F6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="G6">
+        <v>11</v>
+      </c>
+      <c r="H6">
+        <v>180</v>
+      </c>
+      <c r="I6" s="6">
+        <v>41684</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>132</v>
       </c>
@@ -3087,13 +3136,22 @@
         <v>186</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="F7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <v>150</v>
+      </c>
+      <c r="I7" s="6">
+        <v>41680</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>133</v>
       </c>
@@ -3107,13 +3165,13 @@
         <v>186</v>
       </c>
       <c r="E8">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>135</v>
       </c>
@@ -3127,29 +3185,46 @@
         <v>186</v>
       </c>
       <c r="E9">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="F9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+      <c r="G9">
+        <v>16</v>
+      </c>
+      <c r="H9">
+        <v>180</v>
+      </c>
+      <c r="I9" s="6">
+        <v>41687</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="E10">
         <f>SUM(E2:E9)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="G10">
+        <f>SUM(G2:G9)</f>
+        <v>68</v>
+      </c>
+      <c r="H10">
+        <f>SUM(H2:H9)</f>
+        <v>535</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B17" s="5"/>
       <c r="I17" s="7"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B18" s="5"/>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B22" s="5"/>
     </row>
   </sheetData>
@@ -3160,16 +3235,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3196,6 +3274,90 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -3206,16 +3368,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3251,16 +3413,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3296,20 +3458,20 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>110</v>
       </c>
@@ -3320,7 +3482,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>111</v>
       </c>
@@ -3331,7 +3493,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>112</v>
       </c>
@@ -3342,7 +3504,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>113</v>
       </c>
@@ -3353,7 +3515,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -3364,7 +3526,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>115</v>
       </c>
@@ -3375,7 +3537,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>116</v>
       </c>
@@ -3386,7 +3548,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>117</v>
       </c>
@@ -3397,7 +3559,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>118</v>
       </c>
@@ -3408,7 +3570,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>119</v>
       </c>
@@ -3419,7 +3581,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>120</v>
       </c>
@@ -3430,7 +3592,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>121</v>
       </c>
@@ -3441,7 +3603,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>122</v>
       </c>
@@ -3452,7 +3614,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="64" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>123</v>
       </c>
@@ -3463,7 +3625,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>124</v>
       </c>
@@ -3474,7 +3636,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>125</v>
       </c>
@@ -3485,7 +3647,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>126</v>
       </c>
@@ -3496,7 +3658,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>127</v>
       </c>
@@ -3507,7 +3669,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>128</v>
       </c>
@@ -3518,7 +3680,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>129</v>
       </c>
@@ -3529,7 +3691,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>130</v>
       </c>
@@ -3540,7 +3702,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>131</v>
       </c>
@@ -3551,7 +3713,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>132</v>
       </c>
@@ -3562,7 +3724,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>133</v>
       </c>
@@ -3573,7 +3735,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>134</v>
       </c>
@@ -3584,7 +3746,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>135</v>
       </c>
@@ -3595,7 +3757,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="126" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="128" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>136</v>
       </c>
@@ -3606,7 +3768,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>137</v>
       </c>
@@ -3617,7 +3779,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>138</v>
       </c>
@@ -3628,7 +3790,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>139</v>
       </c>
@@ -3639,7 +3801,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>140</v>
       </c>
@@ -3650,7 +3812,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>141</v>
       </c>
@@ -3661,7 +3823,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>142</v>
       </c>
@@ -3672,7 +3834,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>143</v>
       </c>
@@ -3683,7 +3845,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="48" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>144</v>
       </c>
@@ -3694,7 +3856,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>145</v>
       </c>
@@ -3705,7 +3867,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>146</v>
       </c>
@@ -3716,7 +3878,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>147</v>
       </c>
@@ -3727,7 +3889,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>148</v>
       </c>
@@ -3738,7 +3900,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>149</v>
       </c>
@@ -3749,7 +3911,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>150</v>
       </c>
@@ -3760,7 +3922,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>151</v>
       </c>
@@ -3771,7 +3933,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="32" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>152</v>
       </c>

</xml_diff>

<commit_message>
updating excel with user story details
</commit_message>
<xml_diff>
--- a/TeamSSW55AgileMethodsCJBS_Report.xlsx
+++ b/TeamSSW55AgileMethodsCJBS_Report.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sukitha\Documents\GitHub\SSW555AgileMethodsCJBS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacje17\Desktop\assignments\SSW555AgileMethodsCJBS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25695" windowHeight="14565" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25695" windowHeight="14565" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="200">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -667,7 +667,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -911,7 +911,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -973,7 +973,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F4F8-45B3-8E48-DE1D90C4942A}"/>
             </c:ext>
@@ -989,11 +989,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="78186752"/>
-        <c:axId val="78188544"/>
+        <c:axId val="210412960"/>
+        <c:axId val="210413520"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="78186752"/>
+        <c:axId val="210412960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1003,14 +1003,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78188544"/>
+        <c:crossAx val="210413520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="78188544"/>
+        <c:axId val="210413520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1021,7 +1021,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78186752"/>
+        <c:crossAx val="210412960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1039,7 +1039,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1101,7 +1101,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6D39-4E3C-9231-02575099E635}"/>
             </c:ext>
@@ -1117,11 +1117,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="83934592"/>
-        <c:axId val="83960960"/>
+        <c:axId val="210418560"/>
+        <c:axId val="210419120"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="83934592"/>
+        <c:axId val="210418560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1131,14 +1131,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83960960"/>
+        <c:crossAx val="210419120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="83960960"/>
+        <c:axId val="210419120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1149,7 +1149,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83934592"/>
+        <c:crossAx val="210418560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1186,7 +1186,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1224,7 +1224,7 @@
         <xdr:cNvPr id="3" name="Rectangular Callout 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1299,7 +1299,7 @@
         <xdr:cNvPr id="4" name="Rectangular Callout 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1364,7 +1364,7 @@
         <xdr:cNvPr id="5" name="Rectangular Callout 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1433,7 +1433,7 @@
         <xdr:cNvPr id="6" name="Rectangular Callout 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1503,7 +1503,7 @@
         <xdr:cNvPr id="7" name="Rectangular Callout 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1572,7 +1572,7 @@
         <xdr:cNvPr id="8" name="Rectangular Callout 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1642,7 +1642,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1982,7 +1982,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="150" workbookViewId="0">
@@ -2088,10 +2088,10 @@
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="D3" r:id="rId3"/>
+    <hyperlink ref="D4" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2099,11 +2099,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:F18"/>
+    <sheetView topLeftCell="A19" zoomScale="150" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2519,6 +2519,12 @@
       <c r="D31" s="17" t="s">
         <v>183</v>
       </c>
+      <c r="E31" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="F31">
+        <v>3</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
@@ -2533,6 +2539,12 @@
       <c r="D32" s="17" t="s">
         <v>183</v>
       </c>
+      <c r="E32" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
@@ -2559,19 +2571,43 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>3</v>
+      </c>
       <c r="B36" t="s">
         <v>145</v>
       </c>
       <c r="C36" t="s">
         <v>100</v>
       </c>
+      <c r="D36" t="s">
+        <v>183</v>
+      </c>
+      <c r="E36" t="s">
+        <v>186</v>
+      </c>
+      <c r="F36">
+        <v>3</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>3</v>
+      </c>
       <c r="B37" t="s">
         <v>146</v>
       </c>
       <c r="C37" t="s">
         <v>101</v>
+      </c>
+      <c r="D37" t="s">
+        <v>183</v>
+      </c>
+      <c r="E37" t="s">
+        <v>186</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -2654,7 +2690,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
@@ -2842,7 +2878,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
@@ -2981,7 +3017,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
@@ -3283,10 +3319,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -3456,7 +3492,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
@@ -3501,7 +3537,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
@@ -3546,7 +3582,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
@@ -3856,7 +3892,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>137</v>
       </c>

</xml_diff>